<commit_message>
Update fitus Ijazah, Nilai dan Tambah Fitur Data Kurikulum
</commit_message>
<xml_diff>
--- a/template_file/import_ijazah.xlsx
+++ b/template_file/import_ijazah.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sim-kcd9\template_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA9E1584-C7CE-4B84-9538-B2E3F0862D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD31E84-1896-41CB-ADD9-F99FD3E6BDCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAEBBB56-5610-4DF3-8BB1-3C0F32D95CC6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{AAEBBB56-5610-4DF3-8BB1-3C0F32D95CC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Lembar1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>No.</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>DN 123460</t>
+  </si>
+  <si>
+    <t>Jurusan</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>IPS</t>
   </si>
 </sst>
 </file>
@@ -194,7 +203,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -490,128 +499,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97387D1-EC66-4AD3-B697-DBB3A59343AF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="28.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>2021</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>2021</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>2021</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>2021</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>2021</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>